<commit_message>
Definir modelo de calidad y clasificación de issues
</commit_message>
<xml_diff>
--- a/Informes de avance/registro-horas.xlsx
+++ b/Informes de avance/registro-horas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f\Documents\ACTUAL\ISA2\Material\Informes de avance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E1DB2DF-73CC-4CE2-B908-02C8FBE7D00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C021B70B-7E76-4E5F-B4E4-0E0B59F74E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7E97BE49-E50B-4BF4-988E-485098D0788B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Descripción</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Nahuel, Sofía, Fiorella</t>
+  </si>
+  <si>
+    <t>Definición del modelo de calidad, clasificación de issues</t>
+  </si>
+  <si>
+    <t>Definición de estrategias de git branching y estándares de nomenclatura</t>
+  </si>
+  <si>
+    <t>Definición del modelo de calidad y creación de issues</t>
   </si>
 </sst>
 </file>
@@ -449,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89486EB4-4CA2-4A48-BCC4-C64DD37F045F}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,6 +497,66 @@
       <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="3" spans="1:4" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5">
+        <v>45757</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>45759</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5">
+        <v>45760</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -714,20 +783,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0f9474fc-7962-4778-b9b5-9c7319d151e0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0f9474fc-7962-4778-b9b5-9c7319d151e0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -750,14 +819,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F6B5A1-5924-4BBE-BA36-2E6C717205E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5FC5755-3F9C-4FBC-83D5-66EAD970083E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -772,4 +833,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F6B5A1-5924-4BBE-BA36-2E6C717205E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>